<commit_message>
Handle board information on going.
</commit_message>
<xml_diff>
--- a/Bridge_Database/External_File/Documents/Data_Structure.xlsx
+++ b/Bridge_Database/External_File/Documents/Data_Structure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980"/>
   </bookViews>
   <sheets>
     <sheet name="BOARDS" sheetId="1" r:id="rId1"/>
@@ -972,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -982,7 +982,8 @@
     <col min="2" max="2" width="30.75" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="1"/>
+    <col min="5" max="5" width="13.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1203,7 +1204,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:C18"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1438,8 +1439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>